<commit_message>
Refined the Microsoft Excel spreadsheet containing the dataset
</commit_message>
<xml_diff>
--- a/top_50_fast_food_chains_dataset.xlsx
+++ b/top_50_fast_food_chains_dataset.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cervantes\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E51041-450A-4F58-9DA9-74370AD0E3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C4F5C-ED19-48E5-B9E4-ED1FA8B8D6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F564472E-28B7-4795-8192-D31C3E94A4F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Top 50 Fast-Food Chains in USA" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Top 50 Fast-Food Chains in USA'!$A$1:$G$51</definedName>
@@ -254,9 +253,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,7 +644,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -669,7 +667,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
@@ -692,7 +690,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -715,7 +713,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
@@ -738,7 +736,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
@@ -761,7 +759,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
@@ -784,7 +782,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
@@ -807,7 +805,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
@@ -830,7 +828,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
@@ -853,7 +851,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
@@ -876,7 +874,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12">
@@ -899,7 +897,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
@@ -922,7 +920,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
@@ -945,7 +943,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
@@ -968,7 +966,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16">
@@ -991,7 +989,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17">
@@ -1014,7 +1012,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18">
@@ -1037,7 +1035,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19">
@@ -1060,7 +1058,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20">
@@ -1083,7 +1081,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
@@ -1106,7 +1104,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
@@ -1129,7 +1127,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
@@ -1152,7 +1150,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
@@ -1175,7 +1173,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
@@ -1198,7 +1196,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26">
@@ -1221,7 +1219,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27">
@@ -1244,7 +1242,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28">
@@ -1267,7 +1265,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29">
@@ -1290,7 +1288,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30">
@@ -1313,7 +1311,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
       <c r="B31">
@@ -1336,7 +1334,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="B32">
@@ -1359,7 +1357,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33">
@@ -1382,7 +1380,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34">
@@ -1405,7 +1403,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
       <c r="B35">
@@ -1428,7 +1426,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
       <c r="B36">
@@ -1451,7 +1449,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
       <c r="B37">
@@ -1474,7 +1472,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>43</v>
       </c>
       <c r="B38">
@@ -1497,7 +1495,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
       <c r="B39">
@@ -1520,7 +1518,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>45</v>
       </c>
       <c r="B40">
@@ -1543,7 +1541,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41">
@@ -1566,7 +1564,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>47</v>
       </c>
       <c r="B42">
@@ -1589,7 +1587,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43">
@@ -1612,7 +1610,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>49</v>
       </c>
       <c r="B44">
@@ -1635,7 +1633,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
       <c r="B45">
@@ -1658,7 +1656,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
       <c r="B46">
@@ -1681,7 +1679,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>52</v>
       </c>
       <c r="B47">
@@ -1704,7 +1702,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>53</v>
       </c>
       <c r="B48">
@@ -1727,7 +1725,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>54</v>
       </c>
       <c r="B49">
@@ -1750,7 +1748,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>55</v>
       </c>
       <c r="B50">
@@ -1773,7 +1771,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>56</v>
       </c>
       <c r="B51">
@@ -1800,18 +1798,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573ECB68-F163-46FC-8E21-EB9FC1D5C568}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>